<commit_message>
update intro level design
</commit_message>
<xml_diff>
--- a/design_work/level/intro_level.xlsx
+++ b/design_work/level/intro_level.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiji\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Evan_Toronto\2018_2019\GDDC\projectX\design_work\level\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26719182-E908-4A0F-9FE6-DC0746F39A2E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9777F4F9-35E2-4BD6-9843-19DBCCF36EDB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{B7FDA2F1-D0C4-4224-9A04-2A3CFF9BC184}"/>
   </bookViews>
@@ -30,16 +30,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Player Start Point</t>
+  </si>
+  <si>
+    <t>Wall</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Pistol</t>
+  </si>
+  <si>
+    <t>Training Room</t>
+  </si>
+  <si>
+    <t>Pistol Ammo</t>
+  </si>
+  <si>
+    <t>Gate</t>
+  </si>
+  <si>
+    <t>Position for shooting</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Message Point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,13 +76,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="8" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +111,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -145,33 +221,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -488,171 +609,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827DFF9E-E3F4-4156-A5D3-1BA3865E8772}">
-  <dimension ref="D2:Y18"/>
+  <dimension ref="D2:AO28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="4.28515625" style="5"/>
+    <col min="1" max="16384" width="4.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-    </row>
-    <row r="3" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="2" t="s">
+    <row r="2" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="3"/>
+      <c r="K2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="15"/>
+      <c r="AN2" s="15"/>
+      <c r="AO2" s="15"/>
+    </row>
+    <row r="3" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="1"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="13"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
+      <c r="T3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="8"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="7"/>
-      <c r="F4" s="9"/>
-      <c r="H4" s="7"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-    </row>
-    <row r="9" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="4:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="4:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="4:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="7"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="15"/>
+      <c r="AE3" s="15"/>
+      <c r="AF3" s="15"/>
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="15"/>
+      <c r="AI3" s="15"/>
+      <c r="AJ3" s="15"/>
+      <c r="AK3" s="15"/>
+      <c r="AL3" s="15"/>
+      <c r="AM3" s="15"/>
+      <c r="AN3" s="15"/>
+      <c r="AO3" s="15"/>
+    </row>
+    <row r="4" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="4"/>
+      <c r="F4" s="14">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="8"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="7"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="15"/>
+      <c r="AN4" s="15"/>
+      <c r="AO4" s="15"/>
+    </row>
+    <row r="5" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" s="8"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="15"/>
+      <c r="AO5" s="15"/>
+    </row>
+    <row r="6" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="15"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="15"/>
+      <c r="AN6" s="15"/>
+      <c r="AO6" s="15"/>
+    </row>
+    <row r="7" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+      <c r="K9" s="16"/>
+      <c r="U9" s="4"/>
+    </row>
+    <row r="10" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+      <c r="F10" s="12"/>
+      <c r="H10" s="11"/>
+      <c r="J10" s="24">
+        <v>2</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="M10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="U10" s="4"/>
+    </row>
+    <row r="11" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+      <c r="K11" s="16"/>
+      <c r="U11" s="4"/>
+    </row>
+    <row r="12" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="AE12" s="4"/>
+    </row>
+    <row r="13" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="M13" s="22"/>
+      <c r="P13" s="17"/>
+      <c r="S13" s="22"/>
+      <c r="U13" s="4"/>
+      <c r="AE13" s="4"/>
+    </row>
+    <row r="14" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="AE14" s="4"/>
+    </row>
+    <row r="15" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="AE15" s="4"/>
+    </row>
+    <row r="16" spans="4:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="M16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="U16" s="4"/>
+      <c r="AE16" s="4"/>
+    </row>
+    <row r="17" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="AE17" s="4"/>
+    </row>
+    <row r="18" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="4"/>
+      <c r="AE18" s="4"/>
+    </row>
+    <row r="19" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="AE19" s="4"/>
+    </row>
+    <row r="20" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="AE20" s="4"/>
+    </row>
+    <row r="21" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q21" s="4"/>
+      <c r="S21" s="24">
+        <v>3</v>
+      </c>
+      <c r="U21" s="4"/>
+      <c r="AE21" s="4"/>
+    </row>
+    <row r="22" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="AE22" s="4"/>
+    </row>
+    <row r="23" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="AE23" s="4"/>
+    </row>
+    <row r="24" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="AE24" s="4"/>
+    </row>
+    <row r="25" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q25" s="4"/>
+      <c r="AE25" s="4"/>
+    </row>
+    <row r="26" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q26" s="4"/>
+      <c r="AE26" s="4"/>
+    </row>
+    <row r="27" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q27" s="4"/>
+      <c r="AE27" s="4"/>
+    </row>
+    <row r="28" spans="4:31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+      <c r="AE28" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="M3:Q3"/>
+  <mergeCells count="10">
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>